<commit_message>
Added tests and fixed errors
</commit_message>
<xml_diff>
--- a/extracted_SNP_files/SNPinfo_final.xlsx
+++ b/extracted_SNP_files/SNPinfo_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\AmrPlusPlus_SNP\extracted_SNP_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB7C669-EE12-41AA-AFBE-8DDBA4F9002E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BB10F6-F2D0-408E-8E82-475F8E3F888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2602,54 +2602,6 @@
     <t>MEG_3241</t>
   </si>
   <si>
-    <t>Reg:D409N_PGKLA_CAEKD</t>
-  </si>
-  <si>
-    <t>Reg:R457T_NVEKS_LDRIL</t>
-  </si>
-  <si>
-    <t>Reg:D465Y_RILSS_EIKNM</t>
-  </si>
-  <si>
-    <t>Reg:R447LK_AILPL_GKILN</t>
-  </si>
-  <si>
-    <t>Reg:E466VK_ILSSD_IKNMI</t>
-  </si>
-  <si>
-    <t>Reg:S416A_AEKDP_KSEIF</t>
-  </si>
-  <si>
-    <t>Reg:D426VN_FLVEG_SAGGS</t>
-  </si>
-  <si>
-    <t>Reg:S366VA_LEENP_TARII</t>
-  </si>
-  <si>
-    <t>Reg:L444F_NSQAI_PLRGK</t>
-  </si>
-  <si>
-    <t>Reg:S464T_DRILS_DEIKN</t>
-  </si>
-  <si>
-    <t>Reg:I139R_YLNGK_YKQTY</t>
-  </si>
-  <si>
-    <t>Reg:V130I_LSKWM_AEVYL</t>
-  </si>
-  <si>
-    <t>Reg:V423F_SEIFL_EGDSA</t>
-  </si>
-  <si>
-    <t>Reg:R377G_VDKAL_AQRAR</t>
-  </si>
-  <si>
-    <t>Reg:R389P_AAKKA_ELTRR</t>
-  </si>
-  <si>
-    <t>Reg:E399K_RKSVL_STSLP</t>
-  </si>
-  <si>
     <t>MEG_3242</t>
   </si>
   <si>
@@ -2659,27 +2611,6 @@
     <t>MEG_3243</t>
   </si>
   <si>
-    <t>Reg:N538DK_DRVLK_TEVQA</t>
-  </si>
-  <si>
-    <t>Reg:E540VD_VLKNT_VQAII</t>
-  </si>
-  <si>
-    <t>Reg:T539PN_RVLKN_EVQAI</t>
-  </si>
-  <si>
-    <t>Reg:V340L_GYSES_HTFAN</t>
-  </si>
-  <si>
-    <t>Reg:D500H_YVVEG_SAGGS</t>
-  </si>
-  <si>
-    <t>Mult:Reg:R485C_KLADC_STDPR;Reg:T546M_VQAII_ALGTG</t>
-  </si>
-  <si>
-    <t>Mult:Reg:N538T_DRVLK_TEVQA;Reg:T546M_VQAII_ALGTG</t>
-  </si>
-  <si>
     <t>MEG_3244</t>
   </si>
   <si>
@@ -2725,15 +2656,6 @@
     <t>MEG_3246</t>
   </si>
   <si>
-    <t>Reg:T214IA_YNRRG_RVCFH</t>
-  </si>
-  <si>
-    <t>Reg:R184Q_EVEVA_ERKLY</t>
-  </si>
-  <si>
-    <t>Reg:G124S_TDNGR_IPIEN</t>
-  </si>
-  <si>
     <t>MEG_5783</t>
   </si>
   <si>
@@ -4121,6 +4043,84 @@
   </si>
   <si>
     <t>Non:Q142*_KWGEM_PTAPV</t>
+  </si>
+  <si>
+    <t>Reg:D411N_PGKLA_CSSKD</t>
+  </si>
+  <si>
+    <t>Reg:R459T_NVEKQ_LDKIL</t>
+  </si>
+  <si>
+    <t>Reg:D467Y_KILGY_EIRAM</t>
+  </si>
+  <si>
+    <t>Reg:R449LK_AILPL_GKIMN</t>
+  </si>
+  <si>
+    <t>Reg:E468VK_ILGYE_IRAMI</t>
+  </si>
+  <si>
+    <t>Reg:S418A_SSKDP_ECEIY</t>
+  </si>
+  <si>
+    <t>Reg:D428VN_YLVEG_SAGGS</t>
+  </si>
+  <si>
+    <t>Reg:S368VA_LQENP_VAKMI</t>
+  </si>
+  <si>
+    <t>Reg:L446F_KFQAI_PLRGK</t>
+  </si>
+  <si>
+    <t>Reg:S466T_DKILG_EEIRA</t>
+  </si>
+  <si>
+    <t>Reg:I143R_KRESH_WRQVF</t>
+  </si>
+  <si>
+    <t>Reg:V135I_SEICE_EVKRE</t>
+  </si>
+  <si>
+    <t>Reg:V425F_CEIYL_EGDSA</t>
+  </si>
+  <si>
+    <t>Reg:R379G_LDKSL_ASRAR</t>
+  </si>
+  <si>
+    <t>Reg:R391P_AARKA_ELTRR</t>
+  </si>
+  <si>
+    <t>Reg:E401K_RKSIL_NTSLP</t>
+  </si>
+  <si>
+    <t>Reg:N499DK_DRVLK_TEVQA</t>
+  </si>
+  <si>
+    <t>Reg:E501VD_VLKNT_VQAII</t>
+  </si>
+  <si>
+    <t>Reg:T500PN_RVLKN_EVQAI</t>
+  </si>
+  <si>
+    <t>Reg:V301L_GYSES_HTFAN</t>
+  </si>
+  <si>
+    <t>Reg:D461H_YVVEG_SAGGS</t>
+  </si>
+  <si>
+    <t>Mult:Reg:R446C_KLADC_STDPR;Reg:T507M_VQAII_ALGTG</t>
+  </si>
+  <si>
+    <t>Mult:Reg:N499T_DRVLK_TEVQA;Reg:T507M_VQAII_ALGTG</t>
+  </si>
+  <si>
+    <t>Reg:T174IA_GTESG_EISFL</t>
+  </si>
+  <si>
+    <t>Reg:R141Q_VWLRL_IKRDG</t>
+  </si>
+  <si>
+    <t>Reg:G85S_CDNGR_IPTDI</t>
   </si>
 </sst>
 </file>
@@ -4963,8 +4963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DI268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="D262" sqref="D262"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7940,57 +7940,57 @@
         <v>213</v>
       </c>
       <c r="F96" t="s">
-        <v>860</v>
+        <v>1341</v>
       </c>
       <c r="G96" t="s">
-        <v>861</v>
+        <v>1342</v>
       </c>
       <c r="H96" t="s">
-        <v>862</v>
+        <v>1343</v>
       </c>
       <c r="I96" t="s">
-        <v>863</v>
+        <v>1344</v>
       </c>
       <c r="J96" t="s">
-        <v>864</v>
+        <v>1345</v>
       </c>
       <c r="K96" t="s">
-        <v>865</v>
+        <v>1346</v>
       </c>
       <c r="L96" t="s">
-        <v>866</v>
+        <v>1347</v>
       </c>
       <c r="M96" t="s">
-        <v>867</v>
+        <v>1348</v>
       </c>
       <c r="N96" t="s">
-        <v>868</v>
+        <v>1349</v>
       </c>
       <c r="O96" t="s">
-        <v>869</v>
+        <v>1350</v>
       </c>
       <c r="P96" t="s">
-        <v>870</v>
+        <v>1351</v>
       </c>
       <c r="Q96" t="s">
-        <v>871</v>
+        <v>1352</v>
       </c>
       <c r="R96" t="s">
-        <v>872</v>
+        <v>1353</v>
       </c>
       <c r="S96" t="s">
-        <v>873</v>
+        <v>1354</v>
       </c>
       <c r="T96" t="s">
-        <v>874</v>
+        <v>1355</v>
       </c>
       <c r="U96" t="s">
-        <v>875</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="97" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>876</v>
+        <v>860</v>
       </c>
       <c r="B97" t="s">
         <v>1</v>
@@ -8005,12 +8005,12 @@
         <v>213</v>
       </c>
       <c r="F97" t="s">
-        <v>877</v>
+        <v>861</v>
       </c>
     </row>
     <row r="98" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>878</v>
+        <v>862</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
@@ -8025,30 +8025,30 @@
         <v>213</v>
       </c>
       <c r="F98" t="s">
-        <v>879</v>
+        <v>1357</v>
       </c>
       <c r="G98" t="s">
-        <v>880</v>
+        <v>1358</v>
       </c>
       <c r="H98" t="s">
-        <v>881</v>
+        <v>1359</v>
       </c>
       <c r="I98" t="s">
-        <v>882</v>
+        <v>1360</v>
       </c>
       <c r="J98" t="s">
-        <v>883</v>
+        <v>1361</v>
       </c>
       <c r="K98" t="s">
-        <v>884</v>
+        <v>1362</v>
       </c>
       <c r="L98" t="s">
-        <v>885</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="99" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>886</v>
+        <v>863</v>
       </c>
       <c r="B99" t="s">
         <v>1</v>
@@ -8060,15 +8060,15 @@
         <v>227</v>
       </c>
       <c r="E99" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
       <c r="F99" t="s">
-        <v>888</v>
+        <v>865</v>
       </c>
     </row>
     <row r="100" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>893</v>
+        <v>870</v>
       </c>
       <c r="B100" t="s">
         <v>1</v>
@@ -8080,30 +8080,30 @@
         <v>227</v>
       </c>
       <c r="E100" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
       <c r="F100" t="s">
-        <v>894</v>
+        <v>871</v>
       </c>
       <c r="G100" t="s">
-        <v>895</v>
+        <v>872</v>
       </c>
       <c r="H100" t="s">
-        <v>896</v>
+        <v>873</v>
       </c>
       <c r="I100" t="s">
-        <v>897</v>
+        <v>874</v>
       </c>
       <c r="J100" t="s">
-        <v>898</v>
+        <v>875</v>
       </c>
       <c r="K100" t="s">
-        <v>899</v>
+        <v>876</v>
       </c>
     </row>
     <row r="101" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>900</v>
+        <v>877</v>
       </c>
       <c r="B101" t="s">
         <v>1</v>
@@ -8115,16 +8115,16 @@
         <v>227</v>
       </c>
       <c r="E101" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
       <c r="F101" t="s">
-        <v>901</v>
+        <v>1364</v>
       </c>
       <c r="G101" t="s">
-        <v>902</v>
+        <v>1365</v>
       </c>
       <c r="H101" t="s">
-        <v>903</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="102" spans="1:113" x14ac:dyDescent="0.3">
@@ -8149,30 +8149,30 @@
     </row>
     <row r="103" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>912</v>
+        <v>886</v>
       </c>
       <c r="B103" t="s">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>913</v>
+        <v>887</v>
       </c>
       <c r="D103" t="s">
-        <v>914</v>
+        <v>888</v>
       </c>
       <c r="E103" t="s">
-        <v>915</v>
+        <v>889</v>
       </c>
       <c r="F103" t="s">
-        <v>916</v>
+        <v>890</v>
       </c>
       <c r="G103" t="s">
-        <v>917</v>
+        <v>891</v>
       </c>
     </row>
     <row r="104" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>918</v>
+        <v>892</v>
       </c>
       <c r="B104" t="s">
         <v>1</v>
@@ -8184,39 +8184,39 @@
         <v>29</v>
       </c>
       <c r="E104" t="s">
-        <v>919</v>
+        <v>893</v>
       </c>
       <c r="F104" t="s">
-        <v>920</v>
+        <v>894</v>
       </c>
       <c r="G104" t="s">
-        <v>921</v>
+        <v>895</v>
       </c>
       <c r="H104" t="s">
-        <v>922</v>
+        <v>896</v>
       </c>
       <c r="I104" t="s">
-        <v>923</v>
+        <v>897</v>
       </c>
       <c r="J104" t="s">
-        <v>924</v>
+        <v>898</v>
       </c>
       <c r="K104" t="s">
-        <v>925</v>
+        <v>899</v>
       </c>
       <c r="L104" t="s">
-        <v>926</v>
+        <v>900</v>
       </c>
       <c r="M104" t="s">
-        <v>927</v>
+        <v>901</v>
       </c>
       <c r="N104" t="s">
-        <v>928</v>
+        <v>902</v>
       </c>
     </row>
     <row r="105" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>947</v>
+        <v>921</v>
       </c>
       <c r="B105" t="s">
         <v>1</v>
@@ -8225,27 +8225,27 @@
         <v>28</v>
       </c>
       <c r="D105" t="s">
-        <v>948</v>
+        <v>922</v>
       </c>
       <c r="E105" t="s">
-        <v>949</v>
+        <v>923</v>
       </c>
       <c r="F105" t="s">
-        <v>950</v>
+        <v>924</v>
       </c>
       <c r="G105" t="s">
-        <v>951</v>
+        <v>925</v>
       </c>
       <c r="H105" t="s">
-        <v>952</v>
+        <v>926</v>
       </c>
       <c r="I105" t="s">
-        <v>953</v>
+        <v>927</v>
       </c>
     </row>
     <row r="106" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>957</v>
+        <v>931</v>
       </c>
       <c r="B106" t="s">
         <v>1</v>
@@ -8254,18 +8254,18 @@
         <v>28</v>
       </c>
       <c r="D106" t="s">
-        <v>948</v>
+        <v>922</v>
       </c>
       <c r="E106" t="s">
-        <v>958</v>
+        <v>932</v>
       </c>
       <c r="F106" t="s">
-        <v>959</v>
+        <v>933</v>
       </c>
     </row>
     <row r="107" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>960</v>
+        <v>934</v>
       </c>
       <c r="B107" t="s">
         <v>1</v>
@@ -8274,19 +8274,19 @@
         <v>28</v>
       </c>
       <c r="D107" t="s">
-        <v>948</v>
+        <v>922</v>
       </c>
       <c r="E107" t="s">
-        <v>961</v>
+        <v>935</v>
       </c>
       <c r="F107" t="s">
-        <v>962</v>
+        <v>936</v>
       </c>
       <c r="G107" t="s">
-        <v>963</v>
+        <v>937</v>
       </c>
       <c r="H107" t="s">
-        <v>964</v>
+        <v>938</v>
       </c>
     </row>
     <row r="108" spans="1:113" x14ac:dyDescent="0.3">
@@ -8707,7 +8707,7 @@
     </row>
     <row r="112" spans="1:113" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>965</v>
+        <v>939</v>
       </c>
       <c r="B112" t="s">
         <v>1</v>
@@ -8722,12 +8722,12 @@
         <v>4</v>
       </c>
       <c r="F112" t="s">
-        <v>966</v>
+        <v>940</v>
       </c>
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>967</v>
+        <v>941</v>
       </c>
       <c r="B113" t="s">
         <v>1</v>
@@ -8742,16 +8742,16 @@
         <v>4</v>
       </c>
       <c r="F113" t="s">
-        <v>968</v>
+        <v>942</v>
       </c>
       <c r="G113" t="s">
-        <v>969</v>
+        <v>943</v>
       </c>
       <c r="H113" t="s">
-        <v>970</v>
+        <v>944</v>
       </c>
       <c r="I113" t="s">
-        <v>971</v>
+        <v>945</v>
       </c>
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.3">
@@ -8776,7 +8776,7 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>972</v>
+        <v>946</v>
       </c>
       <c r="B115" t="s">
         <v>1</v>
@@ -8791,10 +8791,10 @@
         <v>4</v>
       </c>
       <c r="F115" t="s">
-        <v>973</v>
+        <v>947</v>
       </c>
       <c r="G115" t="s">
-        <v>974</v>
+        <v>948</v>
       </c>
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.3">
@@ -8819,7 +8819,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>976</v>
+        <v>950</v>
       </c>
       <c r="B117" t="s">
         <v>1</v>
@@ -8828,24 +8828,24 @@
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>977</v>
+        <v>951</v>
       </c>
       <c r="E117" t="s">
-        <v>978</v>
+        <v>952</v>
       </c>
       <c r="F117" t="s">
-        <v>979</v>
+        <v>953</v>
       </c>
       <c r="G117" t="s">
-        <v>980</v>
+        <v>954</v>
       </c>
       <c r="H117" t="s">
-        <v>981</v>
+        <v>955</v>
       </c>
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>985</v>
+        <v>959</v>
       </c>
       <c r="B118" t="s">
         <v>1</v>
@@ -8854,13 +8854,13 @@
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>977</v>
+        <v>951</v>
       </c>
       <c r="E118" t="s">
-        <v>986</v>
+        <v>960</v>
       </c>
       <c r="F118" t="s">
-        <v>987</v>
+        <v>961</v>
       </c>
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.3">
@@ -8938,7 +8938,7 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1007</v>
+        <v>981</v>
       </c>
       <c r="B121" t="s">
         <v>122</v>
@@ -8947,13 +8947,13 @@
         <v>123</v>
       </c>
       <c r="D121" t="s">
-        <v>1008</v>
+        <v>982</v>
       </c>
       <c r="E121" t="s">
-        <v>1009</v>
+        <v>983</v>
       </c>
       <c r="F121" t="s">
-        <v>1010</v>
+        <v>984</v>
       </c>
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.3">
@@ -9214,7 +9214,7 @@
     </row>
     <row r="130" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>1011</v>
+        <v>985</v>
       </c>
       <c r="B130" t="s">
         <v>1</v>
@@ -9226,13 +9226,13 @@
         <v>699</v>
       </c>
       <c r="E130" t="s">
-        <v>1012</v>
+        <v>986</v>
       </c>
       <c r="F130" t="s">
-        <v>1013</v>
+        <v>987</v>
       </c>
       <c r="G130" t="s">
-        <v>1014</v>
+        <v>988</v>
       </c>
     </row>
     <row r="131" spans="1:20" x14ac:dyDescent="0.3">
@@ -9252,12 +9252,12 @@
         <v>700</v>
       </c>
       <c r="F131" t="s">
-        <v>1366</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="132" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>1005</v>
+        <v>979</v>
       </c>
       <c r="B132" t="s">
         <v>1</v>
@@ -9272,7 +9272,7 @@
         <v>9</v>
       </c>
       <c r="F132" t="s">
-        <v>1006</v>
+        <v>980</v>
       </c>
     </row>
     <row r="133" spans="1:20" x14ac:dyDescent="0.3">
@@ -9323,7 +9323,7 @@
     </row>
     <row r="135" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>1028</v>
+        <v>1002</v>
       </c>
       <c r="B135" t="s">
         <v>1</v>
@@ -9338,18 +9338,18 @@
         <v>9</v>
       </c>
       <c r="F135" t="s">
-        <v>1029</v>
+        <v>1003</v>
       </c>
       <c r="G135" t="s">
-        <v>1030</v>
+        <v>1004</v>
       </c>
       <c r="H135" t="s">
-        <v>1031</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="136" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>1033</v>
+        <v>1007</v>
       </c>
       <c r="B136" t="s">
         <v>1</v>
@@ -9364,15 +9364,15 @@
         <v>9</v>
       </c>
       <c r="F136" t="s">
-        <v>1034</v>
+        <v>1008</v>
       </c>
       <c r="G136" t="s">
-        <v>1035</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="137" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>1036</v>
+        <v>1010</v>
       </c>
       <c r="B137" t="s">
         <v>1</v>
@@ -9387,15 +9387,15 @@
         <v>9</v>
       </c>
       <c r="F137" t="s">
-        <v>1037</v>
+        <v>1011</v>
       </c>
       <c r="G137" t="s">
-        <v>1038</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="138" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1039</v>
+        <v>1013</v>
       </c>
       <c r="B138" t="s">
         <v>1</v>
@@ -9410,28 +9410,28 @@
         <v>9</v>
       </c>
       <c r="F138" t="s">
-        <v>1040</v>
+        <v>1014</v>
       </c>
       <c r="G138" t="s">
-        <v>1041</v>
+        <v>1015</v>
       </c>
       <c r="H138" t="s">
-        <v>1042</v>
+        <v>1016</v>
       </c>
       <c r="I138" t="s">
-        <v>1043</v>
+        <v>1017</v>
       </c>
       <c r="J138" t="s">
-        <v>1044</v>
+        <v>1018</v>
       </c>
       <c r="K138" t="s">
-        <v>1045</v>
+        <v>1019</v>
       </c>
       <c r="L138" t="s">
-        <v>1046</v>
+        <v>1020</v>
       </c>
       <c r="M138" t="s">
-        <v>1047</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="139" spans="1:20" x14ac:dyDescent="0.3">
@@ -9485,7 +9485,7 @@
     </row>
     <row r="141" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1048</v>
+        <v>1022</v>
       </c>
       <c r="B141" t="s">
         <v>1</v>
@@ -9508,7 +9508,7 @@
     </row>
     <row r="142" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1049</v>
+        <v>1023</v>
       </c>
       <c r="B142" t="s">
         <v>1</v>
@@ -9531,7 +9531,7 @@
     </row>
     <row r="143" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1050</v>
+        <v>1024</v>
       </c>
       <c r="B143" t="s">
         <v>1</v>
@@ -9554,7 +9554,7 @@
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>1051</v>
+        <v>1025</v>
       </c>
       <c r="B144" t="s">
         <v>1</v>
@@ -9686,7 +9686,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>1052</v>
+        <v>1026</v>
       </c>
       <c r="B150" t="s">
         <v>1</v>
@@ -9841,7 +9841,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>1058</v>
+        <v>1032</v>
       </c>
       <c r="B157" t="s">
         <v>1</v>
@@ -10019,7 +10019,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>990</v>
+        <v>964</v>
       </c>
       <c r="B165" t="s">
         <v>1</v>
@@ -10042,7 +10042,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>988</v>
+        <v>962</v>
       </c>
       <c r="B166" t="s">
         <v>1</v>
@@ -10057,12 +10057,12 @@
         <v>228</v>
       </c>
       <c r="F166" t="s">
-        <v>989</v>
+        <v>963</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>1152</v>
+        <v>1126</v>
       </c>
       <c r="B167" t="s">
         <v>1</v>
@@ -10085,7 +10085,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>1153</v>
+        <v>1127</v>
       </c>
       <c r="B168" t="s">
         <v>1</v>
@@ -10108,7 +10108,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>1154</v>
+        <v>1128</v>
       </c>
       <c r="B169" t="s">
         <v>1</v>
@@ -10123,12 +10123,12 @@
         <v>228</v>
       </c>
       <c r="F169" t="s">
-        <v>989</v>
+        <v>963</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>1155</v>
+        <v>1129</v>
       </c>
       <c r="B170" t="s">
         <v>1</v>
@@ -10151,7 +10151,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>1156</v>
+        <v>1130</v>
       </c>
       <c r="B171" t="s">
         <v>1</v>
@@ -10174,7 +10174,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>1157</v>
+        <v>1131</v>
       </c>
       <c r="B172" t="s">
         <v>1</v>
@@ -10197,7 +10197,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>1158</v>
+        <v>1132</v>
       </c>
       <c r="B173" t="s">
         <v>1</v>
@@ -10266,7 +10266,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>1159</v>
+        <v>1133</v>
       </c>
       <c r="B176" t="s">
         <v>1</v>
@@ -10312,7 +10312,7 @@
     </row>
     <row r="178" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>1160</v>
+        <v>1134</v>
       </c>
       <c r="B178" t="s">
         <v>1</v>
@@ -10335,7 +10335,7 @@
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>1161</v>
+        <v>1135</v>
       </c>
       <c r="B179" t="s">
         <v>1</v>
@@ -10358,7 +10358,7 @@
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>1170</v>
+        <v>1144</v>
       </c>
       <c r="B180" t="s">
         <v>1</v>
@@ -10381,7 +10381,7 @@
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>908</v>
+        <v>882</v>
       </c>
       <c r="B181" t="s">
         <v>1</v>
@@ -10393,15 +10393,15 @@
         <v>8</v>
       </c>
       <c r="E181" t="s">
-        <v>909</v>
+        <v>883</v>
       </c>
       <c r="F181" t="s">
-        <v>910</v>
+        <v>884</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>911</v>
+        <v>885</v>
       </c>
       <c r="B182" t="s">
         <v>1</v>
@@ -10413,7 +10413,7 @@
         <v>8</v>
       </c>
       <c r="E182" t="s">
-        <v>909</v>
+        <v>883</v>
       </c>
       <c r="F182" t="s">
         <v>236</v>
@@ -10424,7 +10424,7 @@
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>889</v>
+        <v>866</v>
       </c>
       <c r="B183" t="s">
         <v>1</v>
@@ -10436,18 +10436,18 @@
         <v>253</v>
       </c>
       <c r="E183" t="s">
-        <v>890</v>
+        <v>867</v>
       </c>
       <c r="F183" t="s">
-        <v>891</v>
+        <v>868</v>
       </c>
       <c r="G183" t="s">
-        <v>892</v>
+        <v>869</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>1171</v>
+        <v>1145</v>
       </c>
       <c r="B184" t="s">
         <v>1</v>
@@ -10459,36 +10459,36 @@
         <v>253</v>
       </c>
       <c r="E184" t="s">
-        <v>1172</v>
+        <v>1146</v>
       </c>
       <c r="F184" t="s">
-        <v>1173</v>
+        <v>1147</v>
       </c>
       <c r="G184" t="s">
-        <v>1174</v>
+        <v>1148</v>
       </c>
       <c r="H184" t="s">
-        <v>1175</v>
+        <v>1149</v>
       </c>
       <c r="I184" t="s">
-        <v>1176</v>
+        <v>1150</v>
       </c>
       <c r="J184" t="s">
-        <v>1177</v>
+        <v>1151</v>
       </c>
       <c r="K184" t="s">
-        <v>1178</v>
+        <v>1152</v>
       </c>
       <c r="L184" t="s">
-        <v>1179</v>
+        <v>1153</v>
       </c>
       <c r="M184" t="s">
-        <v>1180</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>1359</v>
+        <v>1333</v>
       </c>
       <c r="B185" t="s">
         <v>1</v>
@@ -10500,16 +10500,16 @@
         <v>253</v>
       </c>
       <c r="E185" t="s">
-        <v>1360</v>
+        <v>1334</v>
       </c>
       <c r="F185" t="s">
-        <v>1361</v>
+        <v>1335</v>
       </c>
       <c r="G185" t="s">
-        <v>1362</v>
+        <v>1336</v>
       </c>
       <c r="H185" t="s">
-        <v>1363</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.3">
@@ -10552,7 +10552,7 @@
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>1181</v>
+        <v>1155</v>
       </c>
       <c r="B187" t="s">
         <v>1</v>
@@ -10564,27 +10564,27 @@
         <v>253</v>
       </c>
       <c r="E187" t="s">
-        <v>1182</v>
+        <v>1156</v>
       </c>
       <c r="F187" t="s">
-        <v>1183</v>
+        <v>1157</v>
       </c>
       <c r="G187" t="s">
-        <v>1184</v>
+        <v>1158</v>
       </c>
       <c r="H187" t="s">
-        <v>1185</v>
+        <v>1159</v>
       </c>
       <c r="I187" t="s">
-        <v>1186</v>
+        <v>1160</v>
       </c>
       <c r="J187" t="s">
-        <v>1187</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>1188</v>
+        <v>1162</v>
       </c>
       <c r="B188" t="s">
         <v>1</v>
@@ -10596,15 +10596,15 @@
         <v>3</v>
       </c>
       <c r="E188" t="s">
-        <v>1189</v>
+        <v>1163</v>
       </c>
       <c r="F188" t="s">
-        <v>1190</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>1191</v>
+        <v>1165</v>
       </c>
       <c r="B189" t="s">
         <v>1</v>
@@ -10616,24 +10616,24 @@
         <v>3</v>
       </c>
       <c r="E189" t="s">
-        <v>1189</v>
+        <v>1163</v>
       </c>
       <c r="F189" t="s">
-        <v>1192</v>
+        <v>1166</v>
       </c>
       <c r="G189" t="s">
-        <v>1190</v>
+        <v>1164</v>
       </c>
       <c r="H189" t="s">
-        <v>1193</v>
+        <v>1167</v>
       </c>
       <c r="I189" t="s">
-        <v>1194</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>904</v>
+        <v>878</v>
       </c>
       <c r="B190" t="s">
         <v>122</v>
@@ -10642,18 +10642,18 @@
         <v>123</v>
       </c>
       <c r="D190" t="s">
-        <v>905</v>
+        <v>879</v>
       </c>
       <c r="E190" t="s">
-        <v>906</v>
+        <v>880</v>
       </c>
       <c r="F190" t="s">
-        <v>907</v>
+        <v>881</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>1166</v>
+        <v>1140</v>
       </c>
       <c r="B191" t="s">
         <v>1</v>
@@ -10662,21 +10662,21 @@
         <v>2</v>
       </c>
       <c r="D191" t="s">
-        <v>977</v>
+        <v>951</v>
       </c>
       <c r="E191" t="s">
-        <v>1167</v>
+        <v>1141</v>
       </c>
       <c r="F191" t="s">
-        <v>1168</v>
+        <v>1142</v>
       </c>
       <c r="G191" t="s">
-        <v>1169</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>1162</v>
+        <v>1136</v>
       </c>
       <c r="B192" t="s">
         <v>1</v>
@@ -10685,21 +10685,21 @@
         <v>2</v>
       </c>
       <c r="D192" t="s">
-        <v>977</v>
+        <v>951</v>
       </c>
       <c r="E192" t="s">
-        <v>1163</v>
+        <v>1137</v>
       </c>
       <c r="F192" t="s">
-        <v>1164</v>
+        <v>1138</v>
       </c>
       <c r="G192" t="s">
-        <v>1165</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="193" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>1059</v>
+        <v>1033</v>
       </c>
       <c r="B193" t="s">
         <v>1</v>
@@ -10711,285 +10711,285 @@
         <v>353</v>
       </c>
       <c r="E193" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F193" t="s">
+        <v>1035</v>
+      </c>
+      <c r="G193" t="s">
+        <v>1036</v>
+      </c>
+      <c r="H193" t="s">
+        <v>1037</v>
+      </c>
+      <c r="I193" t="s">
+        <v>1038</v>
+      </c>
+      <c r="J193" t="s">
+        <v>1039</v>
+      </c>
+      <c r="K193" t="s">
+        <v>1040</v>
+      </c>
+      <c r="L193" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M193" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N193" t="s">
+        <v>1043</v>
+      </c>
+      <c r="O193" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P193" t="s">
+        <v>1045</v>
+      </c>
+      <c r="Q193" t="s">
+        <v>1046</v>
+      </c>
+      <c r="R193" t="s">
+        <v>1047</v>
+      </c>
+      <c r="S193" t="s">
+        <v>1048</v>
+      </c>
+      <c r="T193" t="s">
+        <v>1049</v>
+      </c>
+      <c r="U193" t="s">
+        <v>1050</v>
+      </c>
+      <c r="V193" t="s">
+        <v>1051</v>
+      </c>
+      <c r="W193" t="s">
+        <v>1052</v>
+      </c>
+      <c r="X193" t="s">
+        <v>1053</v>
+      </c>
+      <c r="Y193" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Z193" t="s">
+        <v>1055</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>1056</v>
+      </c>
+      <c r="AB193" t="s">
+        <v>1057</v>
+      </c>
+      <c r="AC193" t="s">
+        <v>1058</v>
+      </c>
+      <c r="AD193" t="s">
+        <v>1059</v>
+      </c>
+      <c r="AE193" t="s">
         <v>1060</v>
       </c>
-      <c r="F193" t="s">
+      <c r="AF193" t="s">
         <v>1061</v>
       </c>
-      <c r="G193" t="s">
+      <c r="AG193" t="s">
         <v>1062</v>
       </c>
-      <c r="H193" t="s">
+      <c r="AH193" t="s">
         <v>1063</v>
       </c>
-      <c r="I193" t="s">
+      <c r="AI193" t="s">
         <v>1064</v>
       </c>
-      <c r="J193" t="s">
+      <c r="AJ193" t="s">
         <v>1065</v>
       </c>
-      <c r="K193" t="s">
+      <c r="AK193" t="s">
         <v>1066</v>
       </c>
-      <c r="L193" t="s">
+      <c r="AL193" t="s">
         <v>1067</v>
       </c>
-      <c r="M193" t="s">
+      <c r="AM193" t="s">
         <v>1068</v>
       </c>
-      <c r="N193" t="s">
+      <c r="AN193" t="s">
         <v>1069</v>
       </c>
-      <c r="O193" t="s">
+      <c r="AO193" t="s">
         <v>1070</v>
       </c>
-      <c r="P193" t="s">
+      <c r="AP193" t="s">
         <v>1071</v>
       </c>
-      <c r="Q193" t="s">
+      <c r="AQ193" t="s">
         <v>1072</v>
       </c>
-      <c r="R193" t="s">
+      <c r="AR193" t="s">
         <v>1073</v>
       </c>
-      <c r="S193" t="s">
+      <c r="AS193" t="s">
         <v>1074</v>
       </c>
-      <c r="T193" t="s">
+      <c r="AT193" t="s">
         <v>1075</v>
       </c>
-      <c r="U193" t="s">
+      <c r="AU193" t="s">
         <v>1076</v>
       </c>
-      <c r="V193" t="s">
+      <c r="AV193" t="s">
         <v>1077</v>
       </c>
-      <c r="W193" t="s">
+      <c r="AW193" t="s">
         <v>1078</v>
       </c>
-      <c r="X193" t="s">
+      <c r="AX193" t="s">
         <v>1079</v>
       </c>
-      <c r="Y193" t="s">
+      <c r="AY193" t="s">
         <v>1080</v>
       </c>
-      <c r="Z193" t="s">
+      <c r="AZ193" t="s">
         <v>1081</v>
       </c>
-      <c r="AA193" t="s">
+      <c r="BA193" t="s">
         <v>1082</v>
       </c>
-      <c r="AB193" t="s">
+      <c r="BB193" t="s">
         <v>1083</v>
       </c>
-      <c r="AC193" t="s">
+      <c r="BC193" t="s">
         <v>1084</v>
       </c>
-      <c r="AD193" t="s">
+      <c r="BD193" t="s">
         <v>1085</v>
       </c>
-      <c r="AE193" t="s">
+      <c r="BE193" t="s">
         <v>1086</v>
       </c>
-      <c r="AF193" t="s">
+      <c r="BF193" t="s">
         <v>1087</v>
       </c>
-      <c r="AG193" t="s">
+      <c r="BG193" t="s">
         <v>1088</v>
       </c>
-      <c r="AH193" t="s">
+      <c r="BH193" t="s">
         <v>1089</v>
       </c>
-      <c r="AI193" t="s">
+      <c r="BI193" t="s">
         <v>1090</v>
       </c>
-      <c r="AJ193" t="s">
+      <c r="BJ193" t="s">
         <v>1091</v>
       </c>
-      <c r="AK193" t="s">
+      <c r="BK193" t="s">
         <v>1092</v>
       </c>
-      <c r="AL193" t="s">
+      <c r="BL193" t="s">
         <v>1093</v>
       </c>
-      <c r="AM193" t="s">
+      <c r="BM193" t="s">
         <v>1094</v>
       </c>
-      <c r="AN193" t="s">
+      <c r="BN193" t="s">
         <v>1095</v>
       </c>
-      <c r="AO193" t="s">
+      <c r="BO193" t="s">
         <v>1096</v>
       </c>
-      <c r="AP193" t="s">
+      <c r="BP193" t="s">
         <v>1097</v>
       </c>
-      <c r="AQ193" t="s">
+      <c r="BQ193" t="s">
         <v>1098</v>
       </c>
-      <c r="AR193" t="s">
+      <c r="BR193" t="s">
         <v>1099</v>
       </c>
-      <c r="AS193" t="s">
+      <c r="BS193" t="s">
         <v>1100</v>
       </c>
-      <c r="AT193" t="s">
+      <c r="BT193" t="s">
         <v>1101</v>
       </c>
-      <c r="AU193" t="s">
+      <c r="BU193" t="s">
         <v>1102</v>
       </c>
-      <c r="AV193" t="s">
+      <c r="BV193" t="s">
         <v>1103</v>
       </c>
-      <c r="AW193" t="s">
+      <c r="BW193" t="s">
         <v>1104</v>
       </c>
-      <c r="AX193" t="s">
+      <c r="BX193" t="s">
         <v>1105</v>
       </c>
-      <c r="AY193" t="s">
+      <c r="BY193" t="s">
         <v>1106</v>
       </c>
-      <c r="AZ193" t="s">
+      <c r="BZ193" t="s">
         <v>1107</v>
       </c>
-      <c r="BA193" t="s">
+      <c r="CA193" t="s">
         <v>1108</v>
       </c>
-      <c r="BB193" t="s">
+      <c r="CB193" t="s">
         <v>1109</v>
       </c>
-      <c r="BC193" t="s">
+      <c r="CC193" t="s">
         <v>1110</v>
       </c>
-      <c r="BD193" t="s">
+      <c r="CD193" t="s">
         <v>1111</v>
       </c>
-      <c r="BE193" t="s">
+      <c r="CE193" t="s">
         <v>1112</v>
       </c>
-      <c r="BF193" t="s">
+      <c r="CF193" t="s">
         <v>1113</v>
       </c>
-      <c r="BG193" t="s">
+      <c r="CG193" t="s">
         <v>1114</v>
       </c>
-      <c r="BH193" t="s">
+      <c r="CH193" t="s">
         <v>1115</v>
       </c>
-      <c r="BI193" t="s">
+      <c r="CI193" t="s">
         <v>1116</v>
       </c>
-      <c r="BJ193" t="s">
+      <c r="CJ193" t="s">
         <v>1117</v>
       </c>
-      <c r="BK193" t="s">
+      <c r="CK193" t="s">
         <v>1118</v>
       </c>
-      <c r="BL193" t="s">
+      <c r="CL193" t="s">
         <v>1119</v>
       </c>
-      <c r="BM193" t="s">
+      <c r="CM193" t="s">
         <v>1120</v>
       </c>
-      <c r="BN193" t="s">
+      <c r="CN193" t="s">
         <v>1121</v>
       </c>
-      <c r="BO193" t="s">
+      <c r="CO193" t="s">
         <v>1122</v>
       </c>
-      <c r="BP193" t="s">
+      <c r="CP193" t="s">
         <v>1123</v>
       </c>
-      <c r="BQ193" t="s">
+      <c r="CQ193" t="s">
         <v>1124</v>
       </c>
-      <c r="BR193" t="s">
+      <c r="CR193" t="s">
         <v>1125</v>
-      </c>
-      <c r="BS193" t="s">
-        <v>1126</v>
-      </c>
-      <c r="BT193" t="s">
-        <v>1127</v>
-      </c>
-      <c r="BU193" t="s">
-        <v>1128</v>
-      </c>
-      <c r="BV193" t="s">
-        <v>1129</v>
-      </c>
-      <c r="BW193" t="s">
-        <v>1130</v>
-      </c>
-      <c r="BX193" t="s">
-        <v>1131</v>
-      </c>
-      <c r="BY193" t="s">
-        <v>1132</v>
-      </c>
-      <c r="BZ193" t="s">
-        <v>1133</v>
-      </c>
-      <c r="CA193" t="s">
-        <v>1134</v>
-      </c>
-      <c r="CB193" t="s">
-        <v>1135</v>
-      </c>
-      <c r="CC193" t="s">
-        <v>1136</v>
-      </c>
-      <c r="CD193" t="s">
-        <v>1137</v>
-      </c>
-      <c r="CE193" t="s">
-        <v>1138</v>
-      </c>
-      <c r="CF193" t="s">
-        <v>1139</v>
-      </c>
-      <c r="CG193" t="s">
-        <v>1140</v>
-      </c>
-      <c r="CH193" t="s">
-        <v>1141</v>
-      </c>
-      <c r="CI193" t="s">
-        <v>1142</v>
-      </c>
-      <c r="CJ193" t="s">
-        <v>1143</v>
-      </c>
-      <c r="CK193" t="s">
-        <v>1144</v>
-      </c>
-      <c r="CL193" t="s">
-        <v>1145</v>
-      </c>
-      <c r="CM193" t="s">
-        <v>1146</v>
-      </c>
-      <c r="CN193" t="s">
-        <v>1147</v>
-      </c>
-      <c r="CO193" t="s">
-        <v>1148</v>
-      </c>
-      <c r="CP193" t="s">
-        <v>1149</v>
-      </c>
-      <c r="CQ193" t="s">
-        <v>1150</v>
-      </c>
-      <c r="CR193" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="194" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>1195</v>
+        <v>1169</v>
       </c>
       <c r="B194" t="s">
         <v>1</v>
@@ -10998,27 +10998,27 @@
         <v>16</v>
       </c>
       <c r="D194" t="s">
-        <v>1196</v>
+        <v>1170</v>
       </c>
       <c r="E194" t="s">
-        <v>1197</v>
+        <v>1171</v>
       </c>
       <c r="F194" t="s">
-        <v>1198</v>
+        <v>1172</v>
       </c>
       <c r="G194" t="s">
-        <v>1199</v>
+        <v>1173</v>
       </c>
       <c r="H194" t="s">
-        <v>1200</v>
+        <v>1174</v>
       </c>
       <c r="I194" t="s">
-        <v>1201</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="195" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>1202</v>
+        <v>1176</v>
       </c>
       <c r="B195" t="s">
         <v>1</v>
@@ -11030,10 +11030,10 @@
         <v>88</v>
       </c>
       <c r="E195" t="s">
-        <v>1203</v>
+        <v>1177</v>
       </c>
       <c r="F195" t="s">
-        <v>1204</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="196" spans="1:96" x14ac:dyDescent="0.3">
@@ -11114,7 +11114,7 @@
     </row>
     <row r="198" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>1205</v>
+        <v>1179</v>
       </c>
       <c r="B198" t="s">
         <v>1</v>
@@ -11126,15 +11126,15 @@
         <v>377</v>
       </c>
       <c r="E198" t="s">
-        <v>1206</v>
+        <v>1180</v>
       </c>
       <c r="F198" t="s">
-        <v>1207</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="199" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>1208</v>
+        <v>1182</v>
       </c>
       <c r="B199" t="s">
         <v>1</v>
@@ -11149,153 +11149,153 @@
         <v>148</v>
       </c>
       <c r="F199" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G199" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H199" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I199" t="s">
+        <v>1186</v>
+      </c>
+      <c r="J199" t="s">
+        <v>1187</v>
+      </c>
+      <c r="K199" t="s">
+        <v>1188</v>
+      </c>
+      <c r="L199" t="s">
+        <v>1189</v>
+      </c>
+      <c r="M199" t="s">
+        <v>1190</v>
+      </c>
+      <c r="N199" t="s">
+        <v>1191</v>
+      </c>
+      <c r="O199" t="s">
+        <v>1192</v>
+      </c>
+      <c r="P199" t="s">
+        <v>1193</v>
+      </c>
+      <c r="Q199" t="s">
+        <v>1194</v>
+      </c>
+      <c r="R199" t="s">
+        <v>1195</v>
+      </c>
+      <c r="S199" t="s">
+        <v>1196</v>
+      </c>
+      <c r="T199" t="s">
+        <v>1197</v>
+      </c>
+      <c r="U199" t="s">
+        <v>1198</v>
+      </c>
+      <c r="V199" t="s">
+        <v>1199</v>
+      </c>
+      <c r="W199" t="s">
+        <v>1201</v>
+      </c>
+      <c r="X199" t="s">
+        <v>1202</v>
+      </c>
+      <c r="Y199" t="s">
+        <v>1203</v>
+      </c>
+      <c r="Z199" t="s">
+        <v>1204</v>
+      </c>
+      <c r="AA199" t="s">
+        <v>1205</v>
+      </c>
+      <c r="AB199" t="s">
+        <v>1206</v>
+      </c>
+      <c r="AC199" t="s">
+        <v>1207</v>
+      </c>
+      <c r="AD199" t="s">
+        <v>1208</v>
+      </c>
+      <c r="AE199" t="s">
         <v>1209</v>
       </c>
-      <c r="G199" t="s">
+      <c r="AF199" t="s">
         <v>1210</v>
       </c>
-      <c r="H199" t="s">
+      <c r="AG199" t="s">
         <v>1211</v>
       </c>
-      <c r="I199" t="s">
+      <c r="AH199" t="s">
         <v>1212</v>
       </c>
-      <c r="J199" t="s">
+      <c r="AI199" t="s">
         <v>1213</v>
       </c>
-      <c r="K199" t="s">
+      <c r="AJ199" t="s">
         <v>1214</v>
       </c>
-      <c r="L199" t="s">
+      <c r="AK199" t="s">
         <v>1215</v>
       </c>
-      <c r="M199" t="s">
+      <c r="AL199" t="s">
         <v>1216</v>
       </c>
-      <c r="N199" t="s">
+      <c r="AM199" t="s">
         <v>1217</v>
       </c>
-      <c r="O199" t="s">
+      <c r="AN199" t="s">
         <v>1218</v>
       </c>
-      <c r="P199" t="s">
+      <c r="AO199" t="s">
         <v>1219</v>
       </c>
-      <c r="Q199" t="s">
+      <c r="AP199" t="s">
         <v>1220</v>
       </c>
-      <c r="R199" t="s">
+      <c r="AQ199" t="s">
         <v>1221</v>
       </c>
-      <c r="S199" t="s">
+      <c r="AR199" t="s">
         <v>1222</v>
       </c>
-      <c r="T199" t="s">
+      <c r="AS199" t="s">
         <v>1223</v>
       </c>
-      <c r="U199" t="s">
+      <c r="AT199" t="s">
         <v>1224</v>
       </c>
-      <c r="V199" t="s">
+      <c r="AU199" t="s">
         <v>1225</v>
       </c>
-      <c r="W199" t="s">
+      <c r="AV199" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AW199" t="s">
         <v>1227</v>
       </c>
-      <c r="X199" t="s">
+      <c r="AX199" t="s">
         <v>1228</v>
       </c>
-      <c r="Y199" t="s">
-        <v>1229</v>
-      </c>
-      <c r="Z199" t="s">
-        <v>1230</v>
-      </c>
-      <c r="AA199" t="s">
-        <v>1231</v>
-      </c>
-      <c r="AB199" t="s">
-        <v>1232</v>
-      </c>
-      <c r="AC199" t="s">
-        <v>1233</v>
-      </c>
-      <c r="AD199" t="s">
-        <v>1234</v>
-      </c>
-      <c r="AE199" t="s">
-        <v>1235</v>
-      </c>
-      <c r="AF199" t="s">
-        <v>1236</v>
-      </c>
-      <c r="AG199" t="s">
-        <v>1237</v>
-      </c>
-      <c r="AH199" t="s">
-        <v>1238</v>
-      </c>
-      <c r="AI199" t="s">
-        <v>1239</v>
-      </c>
-      <c r="AJ199" t="s">
-        <v>1240</v>
-      </c>
-      <c r="AK199" t="s">
-        <v>1241</v>
-      </c>
-      <c r="AL199" t="s">
-        <v>1242</v>
-      </c>
-      <c r="AM199" t="s">
-        <v>1243</v>
-      </c>
-      <c r="AN199" t="s">
-        <v>1244</v>
-      </c>
-      <c r="AO199" t="s">
-        <v>1245</v>
-      </c>
-      <c r="AP199" t="s">
-        <v>1246</v>
-      </c>
-      <c r="AQ199" t="s">
-        <v>1247</v>
-      </c>
-      <c r="AR199" t="s">
-        <v>1248</v>
-      </c>
-      <c r="AS199" t="s">
-        <v>1249</v>
-      </c>
-      <c r="AT199" t="s">
-        <v>1250</v>
-      </c>
-      <c r="AU199" t="s">
-        <v>1251</v>
-      </c>
-      <c r="AV199" t="s">
-        <v>1252</v>
-      </c>
-      <c r="AW199" t="s">
-        <v>1253</v>
-      </c>
-      <c r="AX199" t="s">
-        <v>1254</v>
-      </c>
       <c r="AY199" t="s">
-        <v>1364</v>
+        <v>1338</v>
       </c>
       <c r="AZ199" t="s">
-        <v>1365</v>
+        <v>1339</v>
       </c>
       <c r="BA199" t="s">
-        <v>1226</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="200" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>1255</v>
+        <v>1229</v>
       </c>
       <c r="B200" t="s">
         <v>1</v>
@@ -11310,15 +11310,15 @@
         <v>148</v>
       </c>
       <c r="F200" t="s">
-        <v>1256</v>
+        <v>1230</v>
       </c>
       <c r="G200" t="s">
-        <v>1257</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="201" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>1258</v>
+        <v>1232</v>
       </c>
       <c r="B201" t="s">
         <v>1</v>
@@ -11357,12 +11357,12 @@
         <v>448</v>
       </c>
       <c r="N201" t="s">
-        <v>1259</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="202" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>1260</v>
+        <v>1234</v>
       </c>
       <c r="B202" t="s">
         <v>1</v>
@@ -11377,33 +11377,33 @@
         <v>148</v>
       </c>
       <c r="F202" t="s">
-        <v>1261</v>
+        <v>1235</v>
       </c>
       <c r="G202" t="s">
-        <v>1262</v>
+        <v>1236</v>
       </c>
       <c r="H202" t="s">
-        <v>1263</v>
+        <v>1237</v>
       </c>
       <c r="I202" t="s">
-        <v>1264</v>
+        <v>1238</v>
       </c>
       <c r="J202" t="s">
-        <v>1265</v>
+        <v>1239</v>
       </c>
       <c r="K202" t="s">
-        <v>1266</v>
+        <v>1240</v>
       </c>
       <c r="L202" t="s">
-        <v>1267</v>
+        <v>1241</v>
       </c>
       <c r="M202" t="s">
-        <v>1268</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="203" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>1269</v>
+        <v>1243</v>
       </c>
       <c r="B203" t="s">
         <v>1</v>
@@ -11429,7 +11429,7 @@
     </row>
     <row r="204" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>1270</v>
+        <v>1244</v>
       </c>
       <c r="B204" t="s">
         <v>1</v>
@@ -11473,7 +11473,7 @@
     </row>
     <row r="205" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>1271</v>
+        <v>1245</v>
       </c>
       <c r="B205" t="s">
         <v>1</v>
@@ -11517,7 +11517,7 @@
     </row>
     <row r="206" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>1272</v>
+        <v>1246</v>
       </c>
       <c r="B206" t="s">
         <v>1</v>
@@ -11543,7 +11543,7 @@
     </row>
     <row r="207" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>1273</v>
+        <v>1247</v>
       </c>
       <c r="B207" t="s">
         <v>1</v>
@@ -11575,7 +11575,7 @@
     </row>
     <row r="208" spans="1:96" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>1274</v>
+        <v>1248</v>
       </c>
       <c r="B208" t="s">
         <v>1</v>
@@ -11590,21 +11590,21 @@
         <v>148</v>
       </c>
       <c r="F208" t="s">
-        <v>1000</v>
+        <v>974</v>
       </c>
       <c r="G208" t="s">
-        <v>1001</v>
+        <v>975</v>
       </c>
       <c r="H208" t="s">
-        <v>1002</v>
+        <v>976</v>
       </c>
       <c r="I208" t="s">
-        <v>1003</v>
+        <v>977</v>
       </c>
     </row>
     <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>1275</v>
+        <v>1249</v>
       </c>
       <c r="B209" t="s">
         <v>1</v>
@@ -11648,7 +11648,7 @@
     </row>
     <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>1276</v>
+        <v>1250</v>
       </c>
       <c r="B210" t="s">
         <v>1</v>
@@ -11692,7 +11692,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>1277</v>
+        <v>1251</v>
       </c>
       <c r="B211" t="s">
         <v>1</v>
@@ -11736,7 +11736,7 @@
     </row>
     <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>1278</v>
+        <v>1252</v>
       </c>
       <c r="B212" t="s">
         <v>1</v>
@@ -11765,7 +11765,7 @@
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>1279</v>
+        <v>1253</v>
       </c>
       <c r="B213" t="s">
         <v>1</v>
@@ -11809,7 +11809,7 @@
     </row>
     <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>1280</v>
+        <v>1254</v>
       </c>
       <c r="B214" t="s">
         <v>1</v>
@@ -11955,7 +11955,7 @@
     </row>
     <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>1281</v>
+        <v>1255</v>
       </c>
       <c r="B218" t="s">
         <v>1</v>
@@ -12043,7 +12043,7 @@
     </row>
     <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>1282</v>
+        <v>1256</v>
       </c>
       <c r="B220" t="s">
         <v>1</v>
@@ -12069,7 +12069,7 @@
     </row>
     <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>1004</v>
+        <v>978</v>
       </c>
       <c r="B221" t="s">
         <v>1</v>
@@ -12113,7 +12113,7 @@
     </row>
     <row r="222" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1283</v>
+        <v>1257</v>
       </c>
       <c r="B222" t="s">
         <v>1</v>
@@ -12230,7 +12230,7 @@
     </row>
     <row r="225" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>999</v>
+        <v>973</v>
       </c>
       <c r="B225" t="s">
         <v>1</v>
@@ -12245,16 +12245,16 @@
         <v>148</v>
       </c>
       <c r="F225" t="s">
-        <v>1000</v>
+        <v>974</v>
       </c>
       <c r="G225" t="s">
-        <v>1001</v>
+        <v>975</v>
       </c>
       <c r="H225" t="s">
-        <v>1002</v>
+        <v>976</v>
       </c>
       <c r="I225" t="s">
-        <v>1003</v>
+        <v>977</v>
       </c>
     </row>
     <row r="226" spans="1:34" x14ac:dyDescent="0.3">
@@ -12652,7 +12652,7 @@
     </row>
     <row r="235" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>991</v>
+        <v>965</v>
       </c>
       <c r="B235" t="s">
         <v>1</v>
@@ -12664,15 +12664,15 @@
         <v>76</v>
       </c>
       <c r="E235" t="s">
-        <v>992</v>
+        <v>966</v>
       </c>
       <c r="F235" t="s">
-        <v>993</v>
+        <v>967</v>
       </c>
     </row>
     <row r="236" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>994</v>
+        <v>968</v>
       </c>
       <c r="B236" t="s">
         <v>1</v>
@@ -12681,16 +12681,16 @@
         <v>2</v>
       </c>
       <c r="D236" t="s">
-        <v>995</v>
+        <v>969</v>
       </c>
       <c r="E236" t="s">
-        <v>996</v>
+        <v>970</v>
       </c>
       <c r="F236" t="s">
-        <v>997</v>
+        <v>971</v>
       </c>
       <c r="G236" t="s">
-        <v>998</v>
+        <v>972</v>
       </c>
     </row>
     <row r="237" spans="1:34" x14ac:dyDescent="0.3">
@@ -12765,7 +12765,7 @@
     </row>
     <row r="239" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1284</v>
+        <v>1258</v>
       </c>
       <c r="B239" t="s">
         <v>1</v>
@@ -12774,24 +12774,24 @@
         <v>555</v>
       </c>
       <c r="D239" t="s">
-        <v>1285</v>
+        <v>1259</v>
       </c>
       <c r="E239" t="s">
-        <v>1286</v>
+        <v>1260</v>
       </c>
       <c r="F239" t="s">
-        <v>1287</v>
+        <v>1261</v>
       </c>
       <c r="G239" t="s">
-        <v>1288</v>
+        <v>1262</v>
       </c>
       <c r="H239" t="s">
-        <v>1289</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="240" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>1290</v>
+        <v>1264</v>
       </c>
       <c r="B240" t="s">
         <v>122</v>
@@ -12800,41 +12800,41 @@
         <v>123</v>
       </c>
       <c r="D240" t="s">
-        <v>905</v>
+        <v>879</v>
       </c>
       <c r="E240" t="s">
-        <v>1291</v>
+        <v>1265</v>
       </c>
       <c r="F240" t="s">
-        <v>1292</v>
+        <v>1266</v>
       </c>
       <c r="G240" t="s">
-        <v>1293</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="241" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>1294</v>
+        <v>1268</v>
       </c>
       <c r="B241" t="s">
         <v>122</v>
       </c>
       <c r="C241" t="s">
-        <v>1295</v>
+        <v>1269</v>
       </c>
       <c r="D241" t="s">
-        <v>1296</v>
+        <v>1270</v>
       </c>
       <c r="E241" t="s">
-        <v>1297</v>
+        <v>1271</v>
       </c>
       <c r="F241" t="s">
-        <v>1298</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="242" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1299</v>
+        <v>1273</v>
       </c>
       <c r="B242" t="s">
         <v>1</v>
@@ -12846,66 +12846,66 @@
         <v>377</v>
       </c>
       <c r="E242" t="s">
-        <v>1300</v>
+        <v>1274</v>
       </c>
       <c r="F242" t="s">
-        <v>1301</v>
+        <v>1275</v>
       </c>
       <c r="G242" t="s">
-        <v>1302</v>
+        <v>1276</v>
       </c>
       <c r="H242" t="s">
-        <v>1303</v>
+        <v>1277</v>
       </c>
       <c r="I242" t="s">
-        <v>1304</v>
+        <v>1278</v>
       </c>
       <c r="J242" t="s">
-        <v>1305</v>
+        <v>1279</v>
       </c>
       <c r="K242" t="s">
-        <v>1306</v>
+        <v>1280</v>
       </c>
       <c r="L242" t="s">
-        <v>1307</v>
+        <v>1281</v>
       </c>
       <c r="M242" t="s">
-        <v>1308</v>
+        <v>1282</v>
       </c>
       <c r="N242" t="s">
-        <v>1309</v>
+        <v>1283</v>
       </c>
       <c r="O242" t="s">
-        <v>1310</v>
+        <v>1284</v>
       </c>
       <c r="P242" t="s">
-        <v>1311</v>
+        <v>1285</v>
       </c>
       <c r="Q242" t="s">
-        <v>1312</v>
+        <v>1286</v>
       </c>
       <c r="R242" t="s">
-        <v>1313</v>
+        <v>1287</v>
       </c>
       <c r="S242" t="s">
-        <v>1314</v>
+        <v>1288</v>
       </c>
       <c r="T242" t="s">
-        <v>1315</v>
+        <v>1289</v>
       </c>
       <c r="U242" t="s">
-        <v>1316</v>
+        <v>1290</v>
       </c>
       <c r="V242" t="s">
-        <v>1317</v>
+        <v>1291</v>
       </c>
       <c r="W242" t="s">
-        <v>1318</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="243" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>929</v>
+        <v>903</v>
       </c>
       <c r="B243" t="s">
         <v>1</v>
@@ -12914,60 +12914,60 @@
         <v>555</v>
       </c>
       <c r="D243" t="s">
-        <v>930</v>
+        <v>904</v>
       </c>
       <c r="E243" t="s">
-        <v>931</v>
+        <v>905</v>
       </c>
       <c r="F243" t="s">
-        <v>932</v>
+        <v>906</v>
       </c>
       <c r="G243" t="s">
-        <v>933</v>
+        <v>907</v>
       </c>
       <c r="H243" t="s">
-        <v>934</v>
+        <v>908</v>
       </c>
       <c r="I243" t="s">
-        <v>935</v>
+        <v>909</v>
       </c>
       <c r="J243" t="s">
-        <v>936</v>
+        <v>910</v>
       </c>
       <c r="K243" t="s">
-        <v>937</v>
+        <v>911</v>
       </c>
       <c r="L243" t="s">
-        <v>938</v>
+        <v>912</v>
       </c>
       <c r="M243" t="s">
-        <v>939</v>
+        <v>913</v>
       </c>
       <c r="N243" t="s">
-        <v>940</v>
+        <v>914</v>
       </c>
       <c r="O243" t="s">
-        <v>941</v>
+        <v>915</v>
       </c>
       <c r="P243" t="s">
-        <v>942</v>
+        <v>916</v>
       </c>
       <c r="Q243" t="s">
-        <v>943</v>
+        <v>917</v>
       </c>
       <c r="R243" t="s">
-        <v>944</v>
+        <v>918</v>
       </c>
       <c r="S243" t="s">
-        <v>945</v>
+        <v>919</v>
       </c>
       <c r="T243" t="s">
-        <v>946</v>
+        <v>920</v>
       </c>
     </row>
     <row r="244" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>954</v>
+        <v>928</v>
       </c>
       <c r="B244" t="s">
         <v>1</v>
@@ -12976,21 +12976,21 @@
         <v>555</v>
       </c>
       <c r="D244" t="s">
+        <v>904</v>
+      </c>
+      <c r="E244" t="s">
+        <v>905</v>
+      </c>
+      <c r="F244" t="s">
+        <v>929</v>
+      </c>
+      <c r="G244" t="s">
         <v>930</v>
-      </c>
-      <c r="E244" t="s">
-        <v>931</v>
-      </c>
-      <c r="F244" t="s">
-        <v>955</v>
-      </c>
-      <c r="G244" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="245" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>1053</v>
+        <v>1027</v>
       </c>
       <c r="B245" t="s">
         <v>1</v>
@@ -13005,21 +13005,21 @@
         <v>658</v>
       </c>
       <c r="F245" t="s">
-        <v>1054</v>
+        <v>1028</v>
       </c>
       <c r="G245" t="s">
-        <v>1055</v>
+        <v>1029</v>
       </c>
       <c r="H245" t="s">
-        <v>1056</v>
+        <v>1030</v>
       </c>
       <c r="I245" t="s">
-        <v>1057</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="246" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>1319</v>
+        <v>1293</v>
       </c>
       <c r="B246" t="s">
         <v>1</v>
@@ -13034,30 +13034,30 @@
         <v>658</v>
       </c>
       <c r="F246" t="s">
-        <v>1320</v>
+        <v>1294</v>
       </c>
       <c r="G246" t="s">
-        <v>1321</v>
+        <v>1295</v>
       </c>
       <c r="H246" t="s">
-        <v>1322</v>
+        <v>1296</v>
       </c>
       <c r="I246" t="s">
-        <v>1323</v>
+        <v>1297</v>
       </c>
       <c r="J246" t="s">
-        <v>1324</v>
+        <v>1298</v>
       </c>
       <c r="K246" t="s">
-        <v>1325</v>
+        <v>1299</v>
       </c>
       <c r="L246" t="s">
-        <v>1326</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>1327</v>
+        <v>1301</v>
       </c>
       <c r="B247" t="s">
         <v>1</v>
@@ -13072,10 +13072,10 @@
         <v>658</v>
       </c>
       <c r="F247" t="s">
-        <v>1328</v>
+        <v>1302</v>
       </c>
       <c r="G247" t="s">
-        <v>1329</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.3">
@@ -13129,7 +13129,7 @@
     </row>
     <row r="250" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>1330</v>
+        <v>1304</v>
       </c>
       <c r="B250" t="s">
         <v>1</v>
@@ -13144,7 +13144,7 @@
         <v>658</v>
       </c>
       <c r="F250" t="s">
-        <v>1331</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="251" spans="1:23" x14ac:dyDescent="0.3">
@@ -13261,7 +13261,7 @@
     </row>
     <row r="253" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1332</v>
+        <v>1306</v>
       </c>
       <c r="B253" t="s">
         <v>1</v>
@@ -13317,7 +13317,7 @@
     </row>
     <row r="254" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>1032</v>
+        <v>1006</v>
       </c>
       <c r="B254" t="s">
         <v>1</v>
@@ -13373,7 +13373,7 @@
     </row>
     <row r="255" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>1027</v>
+        <v>1001</v>
       </c>
       <c r="B255" t="s">
         <v>1</v>
@@ -13391,45 +13391,45 @@
         <v>665</v>
       </c>
       <c r="G255" t="s">
-        <v>1016</v>
+        <v>990</v>
       </c>
       <c r="H255" t="s">
         <v>688</v>
       </c>
       <c r="I255" t="s">
-        <v>1017</v>
+        <v>991</v>
       </c>
       <c r="J255" t="s">
-        <v>1018</v>
+        <v>992</v>
       </c>
       <c r="K255" t="s">
-        <v>1019</v>
+        <v>993</v>
       </c>
       <c r="L255" t="s">
         <v>661</v>
       </c>
       <c r="M255" t="s">
-        <v>1020</v>
+        <v>994</v>
       </c>
       <c r="N255" t="s">
-        <v>1021</v>
+        <v>995</v>
       </c>
       <c r="O255" t="s">
-        <v>1022</v>
+        <v>996</v>
       </c>
       <c r="P255" t="s">
-        <v>1023</v>
+        <v>997</v>
       </c>
       <c r="Q255" t="s">
-        <v>1024</v>
+        <v>998</v>
       </c>
       <c r="R255" t="s">
-        <v>1025</v>
+        <v>999</v>
       </c>
     </row>
     <row r="256" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>1333</v>
+        <v>1307</v>
       </c>
       <c r="B256" t="s">
         <v>1</v>
@@ -13456,13 +13456,13 @@
         <v>664</v>
       </c>
       <c r="J256" t="s">
-        <v>983</v>
+        <v>957</v>
       </c>
       <c r="K256" t="s">
         <v>661</v>
       </c>
       <c r="L256" t="s">
-        <v>984</v>
+        <v>958</v>
       </c>
       <c r="M256" t="s">
         <v>659</v>
@@ -13482,7 +13482,7 @@
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>1334</v>
+        <v>1308</v>
       </c>
       <c r="B257" t="s">
         <v>1</v>
@@ -13538,7 +13538,7 @@
     </row>
     <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>975</v>
+        <v>949</v>
       </c>
       <c r="B258" t="s">
         <v>1</v>
@@ -13594,7 +13594,7 @@
     </row>
     <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>982</v>
+        <v>956</v>
       </c>
       <c r="B259" t="s">
         <v>1</v>
@@ -13621,13 +13621,13 @@
         <v>664</v>
       </c>
       <c r="J259" t="s">
-        <v>983</v>
+        <v>957</v>
       </c>
       <c r="K259" t="s">
         <v>661</v>
       </c>
       <c r="L259" t="s">
-        <v>984</v>
+        <v>958</v>
       </c>
       <c r="M259" t="s">
         <v>659</v>
@@ -13647,7 +13647,7 @@
     </row>
     <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>1026</v>
+        <v>1000</v>
       </c>
       <c r="B260" t="s">
         <v>1</v>
@@ -13665,45 +13665,45 @@
         <v>665</v>
       </c>
       <c r="G260" t="s">
-        <v>1016</v>
+        <v>990</v>
       </c>
       <c r="H260" t="s">
         <v>688</v>
       </c>
       <c r="I260" t="s">
-        <v>1017</v>
+        <v>991</v>
       </c>
       <c r="J260" t="s">
-        <v>1018</v>
+        <v>992</v>
       </c>
       <c r="K260" t="s">
-        <v>1019</v>
+        <v>993</v>
       </c>
       <c r="L260" t="s">
         <v>661</v>
       </c>
       <c r="M260" t="s">
-        <v>1020</v>
+        <v>994</v>
       </c>
       <c r="N260" t="s">
-        <v>1021</v>
+        <v>995</v>
       </c>
       <c r="O260" t="s">
-        <v>1022</v>
+        <v>996</v>
       </c>
       <c r="P260" t="s">
-        <v>1023</v>
+        <v>997</v>
       </c>
       <c r="Q260" t="s">
-        <v>1024</v>
+        <v>998</v>
       </c>
       <c r="R260" t="s">
-        <v>1025</v>
+        <v>999</v>
       </c>
     </row>
     <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>1015</v>
+        <v>989</v>
       </c>
       <c r="B261" t="s">
         <v>1</v>
@@ -13721,45 +13721,45 @@
         <v>665</v>
       </c>
       <c r="G261" t="s">
-        <v>1016</v>
+        <v>990</v>
       </c>
       <c r="H261" t="s">
         <v>688</v>
       </c>
       <c r="I261" t="s">
-        <v>1017</v>
+        <v>991</v>
       </c>
       <c r="J261" t="s">
-        <v>1018</v>
+        <v>992</v>
       </c>
       <c r="K261" t="s">
-        <v>1019</v>
+        <v>993</v>
       </c>
       <c r="L261" t="s">
         <v>661</v>
       </c>
       <c r="M261" t="s">
-        <v>1020</v>
+        <v>994</v>
       </c>
       <c r="N261" t="s">
-        <v>1021</v>
+        <v>995</v>
       </c>
       <c r="O261" t="s">
-        <v>1022</v>
+        <v>996</v>
       </c>
       <c r="P261" t="s">
-        <v>1023</v>
+        <v>997</v>
       </c>
       <c r="Q261" t="s">
-        <v>1024</v>
+        <v>998</v>
       </c>
       <c r="R261" t="s">
-        <v>1025</v>
+        <v>999</v>
       </c>
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>1335</v>
+        <v>1309</v>
       </c>
       <c r="B262" t="s">
         <v>1</v>
@@ -13786,13 +13786,13 @@
         <v>664</v>
       </c>
       <c r="J262" t="s">
-        <v>983</v>
+        <v>957</v>
       </c>
       <c r="K262" t="s">
         <v>661</v>
       </c>
       <c r="L262" t="s">
-        <v>984</v>
+        <v>958</v>
       </c>
       <c r="M262" t="s">
         <v>659</v>
@@ -13812,7 +13812,7 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>1336</v>
+        <v>1310</v>
       </c>
       <c r="B263" t="s">
         <v>1</v>
@@ -13830,45 +13830,45 @@
         <v>665</v>
       </c>
       <c r="G263" t="s">
-        <v>1016</v>
+        <v>990</v>
       </c>
       <c r="H263" t="s">
         <v>688</v>
       </c>
       <c r="I263" t="s">
-        <v>1017</v>
+        <v>991</v>
       </c>
       <c r="J263" t="s">
-        <v>1018</v>
+        <v>992</v>
       </c>
       <c r="K263" t="s">
-        <v>1019</v>
+        <v>993</v>
       </c>
       <c r="L263" t="s">
         <v>661</v>
       </c>
       <c r="M263" t="s">
-        <v>1020</v>
+        <v>994</v>
       </c>
       <c r="N263" t="s">
-        <v>1021</v>
+        <v>995</v>
       </c>
       <c r="O263" t="s">
-        <v>1022</v>
+        <v>996</v>
       </c>
       <c r="P263" t="s">
-        <v>1023</v>
+        <v>997</v>
       </c>
       <c r="Q263" t="s">
-        <v>1024</v>
+        <v>998</v>
       </c>
       <c r="R263" t="s">
-        <v>1025</v>
+        <v>999</v>
       </c>
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>1337</v>
+        <v>1311</v>
       </c>
       <c r="B264" t="s">
         <v>1</v>
@@ -13880,27 +13880,27 @@
         <v>88</v>
       </c>
       <c r="E264" t="s">
-        <v>1338</v>
+        <v>1312</v>
       </c>
       <c r="F264" t="s">
-        <v>1339</v>
+        <v>1313</v>
       </c>
       <c r="G264" t="s">
-        <v>1340</v>
+        <v>1314</v>
       </c>
       <c r="H264" t="s">
-        <v>1341</v>
+        <v>1315</v>
       </c>
       <c r="I264" t="s">
-        <v>1342</v>
+        <v>1316</v>
       </c>
       <c r="J264" t="s">
-        <v>1343</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>1344</v>
+        <v>1318</v>
       </c>
       <c r="B265" t="s">
         <v>1</v>
@@ -13912,15 +13912,15 @@
         <v>88</v>
       </c>
       <c r="E265" t="s">
-        <v>1338</v>
+        <v>1312</v>
       </c>
       <c r="F265" t="s">
-        <v>1345</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>1346</v>
+        <v>1320</v>
       </c>
       <c r="B266" t="s">
         <v>1</v>
@@ -13929,30 +13929,30 @@
         <v>75</v>
       </c>
       <c r="D266" t="s">
-        <v>1347</v>
+        <v>1321</v>
       </c>
       <c r="E266" t="s">
-        <v>1348</v>
+        <v>1322</v>
       </c>
       <c r="F266" t="s">
-        <v>1349</v>
+        <v>1323</v>
       </c>
       <c r="G266" t="s">
-        <v>1350</v>
+        <v>1324</v>
       </c>
       <c r="H266" t="s">
-        <v>1351</v>
+        <v>1325</v>
       </c>
       <c r="I266" t="s">
-        <v>1352</v>
+        <v>1326</v>
       </c>
       <c r="J266" t="s">
-        <v>1353</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>1354</v>
+        <v>1328</v>
       </c>
       <c r="B267" t="s">
         <v>1</v>
@@ -13964,16 +13964,16 @@
         <v>3</v>
       </c>
       <c r="E267" t="s">
-        <v>1355</v>
+        <v>1329</v>
       </c>
       <c r="F267" t="s">
-        <v>1356</v>
+        <v>1330</v>
       </c>
       <c r="G267" t="s">
-        <v>1357</v>
+        <v>1331</v>
       </c>
       <c r="H267" t="s">
-        <v>1358</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.3">
@@ -13997,8 +13997,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DO267">
-    <sortCondition ref="A2:A267"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DO265">
+    <sortCondition ref="A2:A265"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>